<commit_message>
updated blup selection index
</commit_message>
<xml_diff>
--- a/data/Cornell_WinterOatFounders_2024_Headrow_phenotypes.xlsx
+++ b/data/Cornell_WinterOatFounders_2024_Headrow_phenotypes.xlsx
@@ -1,15 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pth7\Documents\Intercrop JLJ\2024_winter\2024_winter_intercrop\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0600E137-B35B-47FB-8D2C-23F08BAB5449}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="12" yWindow="0" windowWidth="23016" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -946,8 +965,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -984,13 +1003,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1028,7 +1055,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -1062,6 +1089,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -1096,9 +1124,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1271,14 +1300,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH97"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O19" sqref="O19"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="33" max="33" width="8.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:34">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1382,7 +1416,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:34">
+    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2024</v>
       </c>
@@ -1471,7 +1505,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:34">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2024</v>
       </c>
@@ -1560,7 +1594,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:34">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2024</v>
       </c>
@@ -1649,7 +1683,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:34">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2024</v>
       </c>
@@ -1738,7 +1772,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:34">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2024</v>
       </c>
@@ -1827,7 +1861,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:34">
+    <row r="7" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2024</v>
       </c>
@@ -1916,7 +1950,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:34">
+    <row r="8" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2024</v>
       </c>
@@ -2005,7 +2039,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:34">
+    <row r="9" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2024</v>
       </c>
@@ -2094,7 +2128,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="10" spans="1:34">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2024</v>
       </c>
@@ -2183,7 +2217,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:34">
+    <row r="11" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2024</v>
       </c>
@@ -2272,7 +2306,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="12" spans="1:34">
+    <row r="12" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2024</v>
       </c>
@@ -2361,7 +2395,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:34">
+    <row r="13" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2024</v>
       </c>
@@ -2450,7 +2484,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:34">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2024</v>
       </c>
@@ -2533,13 +2567,13 @@
         <v>45</v>
       </c>
       <c r="AF14">
-        <v>68.9</v>
+        <v>68.900000000000006</v>
       </c>
       <c r="AG14">
         <v>90</v>
       </c>
     </row>
-    <row r="15" spans="1:34">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2024</v>
       </c>
@@ -2628,7 +2662,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:34">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2024</v>
       </c>
@@ -2714,7 +2748,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="17" spans="1:33">
+    <row r="17" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2024</v>
       </c>
@@ -2803,7 +2837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:33">
+    <row r="18" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2024</v>
       </c>
@@ -2892,7 +2926,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="19" spans="1:33">
+    <row r="19" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2024</v>
       </c>
@@ -2981,7 +3015,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:33">
+    <row r="20" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2024</v>
       </c>
@@ -3070,7 +3104,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:33">
+    <row r="21" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2024</v>
       </c>
@@ -3159,7 +3193,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="22" spans="1:33">
+    <row r="22" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2024</v>
       </c>
@@ -3245,7 +3279,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="23" spans="1:33">
+    <row r="23" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2024</v>
       </c>
@@ -3334,7 +3368,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="24" spans="1:33">
+    <row r="24" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2024</v>
       </c>
@@ -3423,7 +3457,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:33">
+    <row r="25" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2024</v>
       </c>
@@ -3512,7 +3546,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="26" spans="1:33">
+    <row r="26" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>2024</v>
       </c>
@@ -3601,7 +3635,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:33">
+    <row r="27" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>2024</v>
       </c>
@@ -3681,13 +3715,13 @@
         <v>45</v>
       </c>
       <c r="AF27">
-        <v>72.32</v>
+        <v>72.319999999999993</v>
       </c>
       <c r="AG27">
         <v>100</v>
       </c>
     </row>
-    <row r="28" spans="1:33">
+    <row r="28" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2024</v>
       </c>
@@ -3776,7 +3810,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="29" spans="1:33">
+    <row r="29" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>2024</v>
       </c>
@@ -3865,7 +3899,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="1:33">
+    <row r="30" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>2024</v>
       </c>
@@ -3954,7 +3988,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="31" spans="1:33">
+    <row r="31" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>2024</v>
       </c>
@@ -4043,7 +4077,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="32" spans="1:33">
+    <row r="32" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>2024</v>
       </c>
@@ -4129,7 +4163,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="33" spans="1:33">
+    <row r="33" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>2024</v>
       </c>
@@ -4215,7 +4249,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="34" spans="1:33">
+    <row r="34" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>2024</v>
       </c>
@@ -4301,7 +4335,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="35" spans="1:33">
+    <row r="35" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2024</v>
       </c>
@@ -4384,13 +4418,13 @@
         <v>45</v>
       </c>
       <c r="AF35">
-        <v>33.02</v>
+        <v>33.020000000000003</v>
       </c>
       <c r="AG35">
         <v>100</v>
       </c>
     </row>
-    <row r="36" spans="1:33">
+    <row r="36" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>2024</v>
       </c>
@@ -4479,7 +4513,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="37" spans="1:33">
+    <row r="37" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>2024</v>
       </c>
@@ -4568,7 +4602,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="38" spans="1:33">
+    <row r="38" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>2024</v>
       </c>
@@ -4657,7 +4691,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="39" spans="1:33">
+    <row r="39" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>2024</v>
       </c>
@@ -4746,7 +4780,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:33">
+    <row r="40" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>2024</v>
       </c>
@@ -4835,7 +4869,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="41" spans="1:33">
+    <row r="41" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>2024</v>
       </c>
@@ -4924,7 +4958,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="42" spans="1:33">
+    <row r="42" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>2024</v>
       </c>
@@ -5013,7 +5047,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="43" spans="1:33">
+    <row r="43" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>2024</v>
       </c>
@@ -5102,7 +5136,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="44" spans="1:33">
+    <row r="44" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>2024</v>
       </c>
@@ -5191,7 +5225,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="45" spans="1:33">
+    <row r="45" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>2024</v>
       </c>
@@ -5280,7 +5314,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="46" spans="1:33">
+    <row r="46" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>2024</v>
       </c>
@@ -5369,7 +5403,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="47" spans="1:33">
+    <row r="47" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>2024</v>
       </c>
@@ -5458,7 +5492,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="48" spans="1:33">
+    <row r="48" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>2024</v>
       </c>
@@ -5547,7 +5581,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="49" spans="1:33">
+    <row r="49" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>2024</v>
       </c>
@@ -5630,13 +5664,13 @@
         <v>45</v>
       </c>
       <c r="AF49">
-        <v>144.17</v>
+        <v>144.16999999999999</v>
       </c>
       <c r="AG49">
         <v>100</v>
       </c>
     </row>
-    <row r="50" spans="1:33">
+    <row r="50" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>2024</v>
       </c>
@@ -5725,7 +5759,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="51" spans="1:33">
+    <row r="51" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>2024</v>
       </c>
@@ -5811,7 +5845,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="52" spans="1:33">
+    <row r="52" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>2024</v>
       </c>
@@ -5897,7 +5931,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="53" spans="1:33">
+    <row r="53" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>2024</v>
       </c>
@@ -5977,13 +6011,13 @@
         <v>45</v>
       </c>
       <c r="AF53">
-        <v>67.43</v>
+        <v>67.430000000000007</v>
       </c>
       <c r="AG53">
         <v>100</v>
       </c>
     </row>
-    <row r="54" spans="1:33">
+    <row r="54" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>2024</v>
       </c>
@@ -6072,7 +6106,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="55" spans="1:33">
+    <row r="55" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>2024</v>
       </c>
@@ -6161,7 +6195,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="56" spans="1:33">
+    <row r="56" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>2024</v>
       </c>
@@ -6241,13 +6275,13 @@
         <v>45</v>
       </c>
       <c r="AF56">
-        <v>17.15</v>
+        <v>17.149999999999999</v>
       </c>
       <c r="AG56">
         <v>100</v>
       </c>
     </row>
-    <row r="57" spans="1:33">
+    <row r="57" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>2024</v>
       </c>
@@ -6336,7 +6370,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="58" spans="1:33">
+    <row r="58" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>2024</v>
       </c>
@@ -6425,7 +6459,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="59" spans="1:33">
+    <row r="59" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>2024</v>
       </c>
@@ -6511,7 +6545,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="60" spans="1:33">
+    <row r="60" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>2024</v>
       </c>
@@ -6600,7 +6634,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="61" spans="1:33">
+    <row r="61" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>2024</v>
       </c>
@@ -6689,7 +6723,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="62" spans="1:33">
+    <row r="62" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>2024</v>
       </c>
@@ -6778,7 +6812,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="63" spans="1:33">
+    <row r="63" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>2024</v>
       </c>
@@ -6867,7 +6901,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="64" spans="1:33">
+    <row r="64" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>2024</v>
       </c>
@@ -6956,7 +6990,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="65" spans="1:33">
+    <row r="65" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>2024</v>
       </c>
@@ -7045,7 +7079,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="66" spans="1:33">
+    <row r="66" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>2024</v>
       </c>
@@ -7134,7 +7168,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="67" spans="1:33">
+    <row r="67" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>2024</v>
       </c>
@@ -7223,7 +7257,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="68" spans="1:33">
+    <row r="68" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>2024</v>
       </c>
@@ -7312,7 +7346,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="69" spans="1:33">
+    <row r="69" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>2024</v>
       </c>
@@ -7395,13 +7429,13 @@
         <v>45</v>
       </c>
       <c r="AF69">
-        <v>139.23</v>
+        <v>139.22999999999999</v>
       </c>
       <c r="AG69">
         <v>100</v>
       </c>
     </row>
-    <row r="70" spans="1:33">
+    <row r="70" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>2024</v>
       </c>
@@ -7490,7 +7524,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="71" spans="1:33">
+    <row r="71" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>2024</v>
       </c>
@@ -7579,7 +7613,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="72" spans="1:33">
+    <row r="72" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>2024</v>
       </c>
@@ -7668,7 +7702,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="73" spans="1:33">
+    <row r="73" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>2024</v>
       </c>
@@ -7754,7 +7788,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="74" spans="1:33">
+    <row r="74" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>2024</v>
       </c>
@@ -7834,13 +7868,13 @@
         <v>45</v>
       </c>
       <c r="AF74">
-        <v>138.8</v>
+        <v>138.80000000000001</v>
       </c>
       <c r="AG74">
         <v>100</v>
       </c>
     </row>
-    <row r="75" spans="1:33">
+    <row r="75" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>2024</v>
       </c>
@@ -7926,7 +7960,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="76" spans="1:33">
+    <row r="76" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>2024</v>
       </c>
@@ -8012,7 +8046,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="77" spans="1:33">
+    <row r="77" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>2024</v>
       </c>
@@ -8098,7 +8132,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="78" spans="1:33">
+    <row r="78" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>2024</v>
       </c>
@@ -8184,7 +8218,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="79" spans="1:33">
+    <row r="79" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>2024</v>
       </c>
@@ -8273,7 +8307,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="80" spans="1:33">
+    <row r="80" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>2024</v>
       </c>
@@ -8359,7 +8393,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="81" spans="1:33">
+    <row r="81" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>2024</v>
       </c>
@@ -8448,7 +8482,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="82" spans="1:33">
+    <row r="82" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>2024</v>
       </c>
@@ -8537,7 +8571,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="83" spans="1:33">
+    <row r="83" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>2024</v>
       </c>
@@ -8626,7 +8660,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="84" spans="1:33">
+    <row r="84" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>2024</v>
       </c>
@@ -8715,7 +8749,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="85" spans="1:33">
+    <row r="85" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>2024</v>
       </c>
@@ -8804,7 +8838,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="86" spans="1:33">
+    <row r="86" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>2024</v>
       </c>
@@ -8893,7 +8927,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:33">
+    <row r="87" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>2024</v>
       </c>
@@ -8979,7 +9013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:33">
+    <row r="88" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>2024</v>
       </c>
@@ -9068,7 +9102,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="89" spans="1:33">
+    <row r="89" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>2024</v>
       </c>
@@ -9157,7 +9191,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="90" spans="1:33">
+    <row r="90" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>2024</v>
       </c>
@@ -9240,13 +9274,13 @@
         <v>45</v>
       </c>
       <c r="AF90">
-        <v>18.94</v>
+        <v>18.940000000000001</v>
       </c>
       <c r="AG90">
         <v>50</v>
       </c>
     </row>
-    <row r="91" spans="1:33">
+    <row r="91" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>2024</v>
       </c>
@@ -9335,7 +9369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="1:33">
+    <row r="92" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>2024</v>
       </c>
@@ -9424,7 +9458,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="93" spans="1:33">
+    <row r="93" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>2024</v>
       </c>
@@ -9510,7 +9544,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="94" spans="1:33">
+    <row r="94" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>2024</v>
       </c>
@@ -9596,7 +9630,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="95" spans="1:33">
+    <row r="95" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>2024</v>
       </c>
@@ -9682,7 +9716,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="96" spans="1:33">
+    <row r="96" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>2024</v>
       </c>
@@ -9771,7 +9805,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="97" spans="1:33">
+    <row r="97" spans="1:33" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>2024</v>
       </c>

</xml_diff>